<commit_message>
added lake wilson pumped hydro and simple_dr
</commit_message>
<xml_diff>
--- a/database/Postgresql Table Creation Scripts/EV simple projections.xlsx
+++ b/database/Postgresql Table Creation Scripts/EV simple projections.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2540" windowWidth="24460" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="5500" yWindow="2320" windowWidth="24460" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1659,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>